<commit_message>
单调练习 Signed-off-by: qingxue0606 <77055664@qq.com>
</commit_message>
<xml_diff>
--- a/音调练习.xlsx
+++ b/音调练习.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6540" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="练" sheetId="3" r:id="rId1"/>
@@ -16,17 +16,17 @@
     <sheet name="七级和弦" sheetId="11" r:id="rId7"/>
     <sheet name="五音阶" sheetId="12" r:id="rId8"/>
     <sheet name="和声学概念" sheetId="10" r:id="rId9"/>
+    <sheet name="大调完全功能" sheetId="13" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">练!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="649">
   <si>
     <t>D</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1482,10 +1482,6 @@
   </si>
   <si>
     <t>增五度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全音-全音-半音-全音-半音-增二度-半音</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2428,6 +2424,382 @@
   </si>
   <si>
     <t>中音 下中音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第36 大调完全功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个正三和弦的上方三度和下方三度都有一个副三和弦，副三和弦与正三和弦功能上近似</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以正三和弦为中心，加上上下三个副三和弦，构成一个功能组，并以正三和弦功能命名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下属功能组和属功能组中各有一个三和弦属于主功能组，形成了各功能之间的联系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>属功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下属功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSVI T DTIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SII S TSVI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTIII D DVII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第37讲 主，属及下属功能组特点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>属功能组所有和弦都有导音，形成这个功能组所固有的紧张性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下属功能组所有的和弦都有六级音，没有导音那样的倾向性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主功能组占有特殊地位，其两个副三和弦都是另外两个功能组组成部分，使得这两个和弦，在功能上具有中间性，根据不同的和弦环境可变现出不同的功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTIII -S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTIII 带有主功能性质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTIII -T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTIII 带有属功能性质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSVI-K46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSVI 带有下属功能性质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-TSVI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSVI 带有主功能性质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第38讲 和声小调的完全功能体系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在小调中加入D的大三和弦，就形成了和声小调，使得大调和小调的和弦在功能有相似之外</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTIII是增三和弦，有着独特的音响，所以未列入主功能组，但由于不稳定性，仍列入属功能组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第39 副三和弦代替正三和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-&gt;TSVI-&gt;S-&gt;SII-&gt;D-&gt;DVII-&gt;T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果在自然小调中，三级三和弦明显属于主功能，而六级三和弦明显属于下属功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>T-&gt;TSVI-&gt;S-&gt;SII-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DTIII</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt;T</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-&gt;TSVI-&gt;S-&gt;SII-&gt;D-&gt;T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公式中每个功能都可以由该功能中的副和弦来代表，代替正三和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副三和弦既可代替正三和弦也可以跟在正三和弦后面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三和弦都可以增加七音变为七和弦，使得音响复杂化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D组的D7，S级的SII7，只有一个音同主和弦，而DVII7更是不含任何主和弦的音，称为主要的七和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更丰富的正格及变格终止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采用完全功能体系中的各个和弦，可以使终止构成更具多样化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每一个功能组中的副三和弦都可以代替或者延伸下厨和弦的进行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正格终止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-D7-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-DVII-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-D7-DTIII-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变格终止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-S-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-TSVI-S-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-TSVI-S-SII-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完全终止拓展</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-TSVI-S-Sii-DVII-D7-DTIII6-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>41讲 二级六和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>II级六和弦是所有副三和弦中应用得最广的弦，也是下属功能组最常用的代表和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在古典音乐中，甚至比下属和弦使用还要多，其功能上有强烈的不稳定性，还具有小调色彩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四部和声中主要重复低音，用来代替下属和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般放在T或者S后，上三声部与低音反向进行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>42讲 二级七和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二级七和弦使用的最多的是第一转位五六和弦，也成为附加六度音的下属和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SII7一般也是解决到属和弦，当连接D时，五，七音级进下行，三音在转位和弦中做级进上行，原位和弦中常做三度下行，根音如在低音部则跳进至D4的根音，在上方三声部则保持不动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>43 六级三和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副三和弦当中，除了SII以外用的最多的就是大调与小调的六级三和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当六级和弦在T和S中间，其功能被模糊化，成了两者之间的中间环节；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>当原位TSVI放在D或者D7后面，它就近似于主功能，称之</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>阻碍进行，之后可连接到各功能组的和弦；</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44讲六级三和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSVI放在D或者K46之前，，也就是典型的S所在的位置，便具有了下属属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当阻碍进行使用在终止中，变成了阻碍终止，可以使终止乐句延长结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在乐段结尾使用三音或者五音旋律位置或将主和弦入到弱拍上，形成不完满终止，可继续进行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在结束终止时，在D或者K46后使用D2，从而解决到T6，可再继续进行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全音-全音-半音-全音-半音-增二度-半音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>45 和声大调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将自然大调的六级音降半音，就成了和声大调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和声大调的四级及二级和弦与同主间小调一样，且二级和弦一般只有六和弦，六级增三和弦很少用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>半音进行如果跨声部进行，称为对斜关系，目前在本课程中禁止使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>46导七和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在七级音上的七和弦成为导七和弦，它具有属功能，标记DVII7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导七和弦常使用在主和弦之后，也作为经过性质的和弦用在下属功能组的和弦后面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DVII的第二转位和弦具有较强的下属功能特征，可作为S的替代和弦直接进行变格终止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-&gt;DVII7     S-&gt;DVII56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T-&gt;TSVI-&gt;DVII34-&gt;T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>47属九和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D7上再加一个三度，就是属九，标记D9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C大调中是大属九和弦，小调与和声小调是小属九和弦，属九和弦几乎使用原位和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>属九和弦在排列时，其根音和九音需处在不同八度音区中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>属九和弦在与下属和弦连接时，一般保持共同音不变（七音和九音），一般省略5音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>48讲 二级九和弦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二级九，就是二级七的复杂版本，连接最多到属，也可到主</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二级和弦上建立的九和弦，标记SII9，主要使用在大调当中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果使用不完全的二级九和弦，一般也是省略五音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SII7及其转位主要用于代替简单的下属和弦S与SII，七音一般不出现在旋律声部。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2722,7 +3094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2809,6 +3181,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3152,7 +3531,7 @@
         <v>48</v>
       </c>
       <c r="X1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3186,7 +3565,7 @@
         <v>161</v>
       </c>
       <c r="X2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3217,7 +3596,7 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3248,7 +3627,7 @@
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3282,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="X5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3311,7 +3690,7 @@
         <v>2</v>
       </c>
       <c r="X6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="21" thickTop="1" x14ac:dyDescent="0.25">
@@ -3349,7 +3728,7 @@
         <v>1</v>
       </c>
       <c r="X7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3383,7 +3762,7 @@
         <v>1</v>
       </c>
       <c r="X8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3417,7 +3796,7 @@
         <v>2</v>
       </c>
       <c r="X9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3451,7 +3830,7 @@
         <v>1</v>
       </c>
       <c r="X10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3485,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="X11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -3501,7 +3880,7 @@
         <v>1</v>
       </c>
       <c r="X12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3539,7 +3918,7 @@
         <v>2</v>
       </c>
       <c r="X13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3564,7 +3943,7 @@
         <v>49</v>
       </c>
       <c r="X14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3589,7 +3968,7 @@
         <v>50</v>
       </c>
       <c r="X15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3617,34 +3996,34 @@
         <v>220</v>
       </c>
       <c r="M16" t="s">
+        <v>433</v>
+      </c>
+      <c r="N16" t="s">
+        <v>437</v>
+      </c>
+      <c r="O16" t="s">
         <v>434</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>436</v>
+      </c>
+      <c r="R16" t="s">
         <v>438</v>
       </c>
-      <c r="O16" t="s">
+      <c r="S16" t="s">
         <v>435</v>
       </c>
-      <c r="P16" t="s">
+      <c r="T16" t="s">
         <v>433</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="U16" t="s">
         <v>437</v>
       </c>
-      <c r="R16" t="s">
-        <v>439</v>
-      </c>
-      <c r="S16" t="s">
-        <v>436</v>
-      </c>
-      <c r="T16" t="s">
-        <v>434</v>
-      </c>
-      <c r="U16" t="s">
-        <v>438</v>
-      </c>
       <c r="X16" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3672,34 +4051,34 @@
         <v>221</v>
       </c>
       <c r="M17" t="s">
+        <v>434</v>
+      </c>
+      <c r="N17" t="s">
+        <v>432</v>
+      </c>
+      <c r="O17" t="s">
+        <v>436</v>
+      </c>
+      <c r="P17" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q17" t="s">
         <v>435</v>
       </c>
-      <c r="N17" t="s">
+      <c r="R17" t="s">
         <v>433</v>
       </c>
-      <c r="O17" t="s">
+      <c r="S17" t="s">
         <v>437</v>
       </c>
-      <c r="P17" t="s">
-        <v>439</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>436</v>
-      </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>434</v>
       </c>
-      <c r="S17" t="s">
-        <v>438</v>
-      </c>
-      <c r="T17" t="s">
-        <v>435</v>
-      </c>
       <c r="U17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="X17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3725,34 +4104,34 @@
         <v>222</v>
       </c>
       <c r="M18" t="s">
+        <v>436</v>
+      </c>
+      <c r="N18" t="s">
+        <v>438</v>
+      </c>
+      <c r="O18" t="s">
+        <v>435</v>
+      </c>
+      <c r="P18" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q18" t="s">
         <v>437</v>
       </c>
-      <c r="N18" t="s">
+      <c r="R18" t="s">
+        <v>434</v>
+      </c>
+      <c r="S18" t="s">
+        <v>432</v>
+      </c>
+      <c r="T18" t="s">
+        <v>436</v>
+      </c>
+      <c r="U18" t="s">
         <v>439</v>
       </c>
-      <c r="O18" t="s">
-        <v>436</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="X18" t="s">
         <v>434</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>438</v>
-      </c>
-      <c r="R18" t="s">
-        <v>435</v>
-      </c>
-      <c r="S18" t="s">
-        <v>433</v>
-      </c>
-      <c r="T18" t="s">
-        <v>437</v>
-      </c>
-      <c r="U18" t="s">
-        <v>440</v>
-      </c>
-      <c r="X18" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="21" thickTop="1" x14ac:dyDescent="0.25">
@@ -3784,34 +4163,34 @@
         <v>223</v>
       </c>
       <c r="M19" t="s">
+        <v>435</v>
+      </c>
+      <c r="N19" t="s">
+        <v>433</v>
+      </c>
+      <c r="O19" t="s">
+        <v>437</v>
+      </c>
+      <c r="P19" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>432</v>
+      </c>
+      <c r="R19" t="s">
         <v>436</v>
       </c>
-      <c r="N19" t="s">
-        <v>434</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="S19" t="s">
         <v>438</v>
       </c>
-      <c r="P19" t="s">
+      <c r="T19" t="s">
         <v>435</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="U19" t="s">
         <v>433</v>
       </c>
-      <c r="R19" t="s">
-        <v>437</v>
-      </c>
-      <c r="S19" t="s">
-        <v>439</v>
-      </c>
-      <c r="T19" t="s">
-        <v>436</v>
-      </c>
-      <c r="U19" t="s">
-        <v>434</v>
-      </c>
       <c r="X19" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3839,34 +4218,34 @@
         <v>224</v>
       </c>
       <c r="M20" t="s">
+        <v>437</v>
+      </c>
+      <c r="N20" t="s">
+        <v>434</v>
+      </c>
+      <c r="O20" t="s">
+        <v>432</v>
+      </c>
+      <c r="P20" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q20" t="s">
         <v>438</v>
       </c>
-      <c r="N20" t="s">
+      <c r="R20" t="s">
         <v>435</v>
       </c>
-      <c r="O20" t="s">
+      <c r="S20" t="s">
         <v>433</v>
       </c>
-      <c r="P20" t="s">
+      <c r="T20" t="s">
         <v>437</v>
       </c>
-      <c r="Q20" t="s">
-        <v>439</v>
-      </c>
-      <c r="R20" t="s">
+      <c r="U20" t="s">
+        <v>434</v>
+      </c>
+      <c r="X20" t="s">
         <v>436</v>
-      </c>
-      <c r="S20" t="s">
-        <v>434</v>
-      </c>
-      <c r="T20" t="s">
-        <v>438</v>
-      </c>
-      <c r="U20" t="s">
-        <v>435</v>
-      </c>
-      <c r="X20" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3894,34 +4273,34 @@
         <v>225</v>
       </c>
       <c r="M21" t="s">
+        <v>432</v>
+      </c>
+      <c r="N21" t="s">
+        <v>436</v>
+      </c>
+      <c r="O21" t="s">
+        <v>438</v>
+      </c>
+      <c r="P21" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q21" t="s">
         <v>433</v>
       </c>
-      <c r="N21" t="s">
+      <c r="R21" t="s">
         <v>437</v>
       </c>
-      <c r="O21" t="s">
-        <v>439</v>
-      </c>
-      <c r="P21" t="s">
+      <c r="S21" t="s">
+        <v>434</v>
+      </c>
+      <c r="T21" t="s">
+        <v>432</v>
+      </c>
+      <c r="U21" t="s">
         <v>436</v>
       </c>
-      <c r="Q21" t="s">
-        <v>434</v>
-      </c>
-      <c r="R21" t="s">
+      <c r="X21" t="s">
         <v>438</v>
-      </c>
-      <c r="S21" t="s">
-        <v>435</v>
-      </c>
-      <c r="T21" t="s">
-        <v>433</v>
-      </c>
-      <c r="U21" t="s">
-        <v>437</v>
-      </c>
-      <c r="X21" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3949,34 +4328,34 @@
         <v>226</v>
       </c>
       <c r="M22" t="s">
+        <v>438</v>
+      </c>
+      <c r="N22" t="s">
+        <v>435</v>
+      </c>
+      <c r="O22" t="s">
+        <v>433</v>
+      </c>
+      <c r="P22" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>434</v>
+      </c>
+      <c r="R22" t="s">
+        <v>432</v>
+      </c>
+      <c r="S22" t="s">
+        <v>436</v>
+      </c>
+      <c r="T22" t="s">
         <v>439</v>
       </c>
-      <c r="N22" t="s">
-        <v>436</v>
-      </c>
-      <c r="O22" t="s">
-        <v>434</v>
-      </c>
-      <c r="P22" t="s">
-        <v>438</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>435</v>
-      </c>
-      <c r="R22" t="s">
-        <v>433</v>
-      </c>
-      <c r="S22" t="s">
-        <v>437</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>440</v>
       </c>
-      <c r="U22" t="s">
+      <c r="X22" t="s">
         <v>441</v>
-      </c>
-      <c r="X22" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4001,14 +4380,14 @@
         <v>51</v>
       </c>
       <c r="X23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="H24" s="10"/>
       <c r="X24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4058,7 +4437,7 @@
         <v>219</v>
       </c>
       <c r="X25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4104,7 +4483,7 @@
         <v>219</v>
       </c>
       <c r="X26" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4150,7 +4529,7 @@
         <v>227</v>
       </c>
       <c r="X27" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4172,7 +4551,7 @@
         <v>6</v>
       </c>
       <c r="X28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4194,7 +4573,7 @@
         <v>4</v>
       </c>
       <c r="X29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4256,7 +4635,7 @@
         <v>5</v>
       </c>
       <c r="M32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4316,17 +4695,17 @@
         <v>6</v>
       </c>
       <c r="M35" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N35" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="H36" s="10"/>
       <c r="M36" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="N36" t="s">
         <v>20</v>
@@ -4355,10 +4734,10 @@
         <v>5</v>
       </c>
       <c r="M37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N37" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -4380,10 +4759,10 @@
         <v>3</v>
       </c>
       <c r="M38" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N38" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -23359,366 +23738,6 @@
     </row>
   </sheetData>
   <mergeCells count="384">
-    <mergeCell ref="A1117:A1121"/>
-    <mergeCell ref="A1123:A1127"/>
-    <mergeCell ref="A1129:A1133"/>
-    <mergeCell ref="A1135:A1139"/>
-    <mergeCell ref="A1141:A1145"/>
-    <mergeCell ref="A1147:A1151"/>
-    <mergeCell ref="A1081:A1085"/>
-    <mergeCell ref="A1087:A1091"/>
-    <mergeCell ref="A1093:A1097"/>
-    <mergeCell ref="A1099:A1103"/>
-    <mergeCell ref="A1105:A1109"/>
-    <mergeCell ref="A1111:A1115"/>
-    <mergeCell ref="A1045:A1049"/>
-    <mergeCell ref="A1051:A1055"/>
-    <mergeCell ref="A1057:A1061"/>
-    <mergeCell ref="A1063:A1067"/>
-    <mergeCell ref="A1069:A1073"/>
-    <mergeCell ref="A1075:A1079"/>
-    <mergeCell ref="A1009:A1013"/>
-    <mergeCell ref="A1015:A1019"/>
-    <mergeCell ref="A1021:A1025"/>
-    <mergeCell ref="A1027:A1031"/>
-    <mergeCell ref="A1033:A1037"/>
-    <mergeCell ref="A1039:A1043"/>
-    <mergeCell ref="A973:A977"/>
-    <mergeCell ref="A979:A983"/>
-    <mergeCell ref="A985:A989"/>
-    <mergeCell ref="A991:A995"/>
-    <mergeCell ref="A997:A1001"/>
-    <mergeCell ref="A1003:A1007"/>
-    <mergeCell ref="A937:A941"/>
-    <mergeCell ref="A943:A947"/>
-    <mergeCell ref="A949:A953"/>
-    <mergeCell ref="A955:A959"/>
-    <mergeCell ref="A961:A965"/>
-    <mergeCell ref="A967:A971"/>
-    <mergeCell ref="A901:A905"/>
-    <mergeCell ref="A907:A911"/>
-    <mergeCell ref="A913:A917"/>
-    <mergeCell ref="A919:A923"/>
-    <mergeCell ref="A925:A929"/>
-    <mergeCell ref="A931:A935"/>
-    <mergeCell ref="A865:A869"/>
-    <mergeCell ref="A871:A875"/>
-    <mergeCell ref="A877:A881"/>
-    <mergeCell ref="A883:A887"/>
-    <mergeCell ref="A889:A893"/>
-    <mergeCell ref="A895:A899"/>
-    <mergeCell ref="A829:A833"/>
-    <mergeCell ref="A835:A839"/>
-    <mergeCell ref="A841:A845"/>
-    <mergeCell ref="A847:A851"/>
-    <mergeCell ref="A853:A857"/>
-    <mergeCell ref="A859:A863"/>
-    <mergeCell ref="A793:A797"/>
-    <mergeCell ref="A799:A803"/>
-    <mergeCell ref="A805:A809"/>
-    <mergeCell ref="A811:A815"/>
-    <mergeCell ref="A817:A821"/>
-    <mergeCell ref="A823:A827"/>
-    <mergeCell ref="A757:A761"/>
-    <mergeCell ref="A763:A767"/>
-    <mergeCell ref="A769:A773"/>
-    <mergeCell ref="A775:A779"/>
-    <mergeCell ref="A781:A785"/>
-    <mergeCell ref="A787:A791"/>
-    <mergeCell ref="A721:A725"/>
-    <mergeCell ref="A727:A731"/>
-    <mergeCell ref="A733:A737"/>
-    <mergeCell ref="A739:A743"/>
-    <mergeCell ref="A745:A749"/>
-    <mergeCell ref="A751:A755"/>
-    <mergeCell ref="A685:A689"/>
-    <mergeCell ref="A691:A695"/>
-    <mergeCell ref="A697:A701"/>
-    <mergeCell ref="A703:A707"/>
-    <mergeCell ref="A709:A713"/>
-    <mergeCell ref="A715:A719"/>
-    <mergeCell ref="A649:A653"/>
-    <mergeCell ref="A655:A659"/>
-    <mergeCell ref="A661:A665"/>
-    <mergeCell ref="A667:A671"/>
-    <mergeCell ref="A673:A677"/>
-    <mergeCell ref="A679:A683"/>
-    <mergeCell ref="A613:A617"/>
-    <mergeCell ref="A619:A623"/>
-    <mergeCell ref="A625:A629"/>
-    <mergeCell ref="A631:A635"/>
-    <mergeCell ref="A637:A641"/>
-    <mergeCell ref="A643:A647"/>
-    <mergeCell ref="A577:A581"/>
-    <mergeCell ref="A583:A587"/>
-    <mergeCell ref="A589:A593"/>
-    <mergeCell ref="A595:A599"/>
-    <mergeCell ref="A601:A605"/>
-    <mergeCell ref="A607:A611"/>
-    <mergeCell ref="A541:A545"/>
-    <mergeCell ref="A547:A551"/>
-    <mergeCell ref="A553:A557"/>
-    <mergeCell ref="A559:A563"/>
-    <mergeCell ref="A565:A569"/>
-    <mergeCell ref="A571:A575"/>
-    <mergeCell ref="A505:A509"/>
-    <mergeCell ref="A511:A515"/>
-    <mergeCell ref="A517:A521"/>
-    <mergeCell ref="A523:A527"/>
-    <mergeCell ref="A529:A533"/>
-    <mergeCell ref="A535:A539"/>
-    <mergeCell ref="A469:A473"/>
-    <mergeCell ref="A475:A479"/>
-    <mergeCell ref="A481:A485"/>
-    <mergeCell ref="A487:A491"/>
-    <mergeCell ref="A493:A497"/>
-    <mergeCell ref="A499:A503"/>
-    <mergeCell ref="A433:A437"/>
-    <mergeCell ref="A439:A443"/>
-    <mergeCell ref="A445:A449"/>
-    <mergeCell ref="A451:A455"/>
-    <mergeCell ref="A457:A461"/>
-    <mergeCell ref="A463:A467"/>
-    <mergeCell ref="A397:A401"/>
-    <mergeCell ref="A403:A407"/>
-    <mergeCell ref="A409:A413"/>
-    <mergeCell ref="A415:A419"/>
-    <mergeCell ref="A421:A425"/>
-    <mergeCell ref="A427:A431"/>
-    <mergeCell ref="A361:A365"/>
-    <mergeCell ref="A367:A371"/>
-    <mergeCell ref="A373:A377"/>
-    <mergeCell ref="A379:A383"/>
-    <mergeCell ref="A385:A389"/>
-    <mergeCell ref="A391:A395"/>
-    <mergeCell ref="A325:A329"/>
-    <mergeCell ref="A331:A335"/>
-    <mergeCell ref="A337:A341"/>
-    <mergeCell ref="A343:A347"/>
-    <mergeCell ref="A349:A353"/>
-    <mergeCell ref="A355:A359"/>
-    <mergeCell ref="A289:A293"/>
-    <mergeCell ref="A295:A299"/>
-    <mergeCell ref="A301:A305"/>
-    <mergeCell ref="A307:A311"/>
-    <mergeCell ref="A313:A317"/>
-    <mergeCell ref="A319:A323"/>
-    <mergeCell ref="A253:A257"/>
-    <mergeCell ref="A259:A263"/>
-    <mergeCell ref="A265:A269"/>
-    <mergeCell ref="A271:A275"/>
-    <mergeCell ref="A277:A281"/>
-    <mergeCell ref="A283:A287"/>
-    <mergeCell ref="A217:A221"/>
-    <mergeCell ref="A223:A227"/>
-    <mergeCell ref="A229:A233"/>
-    <mergeCell ref="A235:A239"/>
-    <mergeCell ref="A241:A245"/>
-    <mergeCell ref="A247:A251"/>
-    <mergeCell ref="A181:A185"/>
-    <mergeCell ref="A187:A191"/>
-    <mergeCell ref="A193:A197"/>
-    <mergeCell ref="A199:A203"/>
-    <mergeCell ref="A205:A209"/>
-    <mergeCell ref="A211:A215"/>
-    <mergeCell ref="A145:A149"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="A157:A161"/>
-    <mergeCell ref="A163:A167"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A175:A179"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="A115:A119"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="A133:A137"/>
-    <mergeCell ref="A139:A143"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="A103:A107"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="G1:G5"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G13:G17"/>
-    <mergeCell ref="G19:G23"/>
-    <mergeCell ref="G25:G29"/>
-    <mergeCell ref="G31:G35"/>
-    <mergeCell ref="G37:G41"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="G55:G59"/>
-    <mergeCell ref="G61:G65"/>
-    <mergeCell ref="G67:G71"/>
-    <mergeCell ref="G73:G77"/>
-    <mergeCell ref="G79:G83"/>
-    <mergeCell ref="G85:G89"/>
-    <mergeCell ref="G91:G95"/>
-    <mergeCell ref="G97:G101"/>
-    <mergeCell ref="G103:G107"/>
-    <mergeCell ref="G109:G113"/>
-    <mergeCell ref="G115:G119"/>
-    <mergeCell ref="G121:G125"/>
-    <mergeCell ref="G127:G131"/>
-    <mergeCell ref="G133:G137"/>
-    <mergeCell ref="G139:G143"/>
-    <mergeCell ref="G145:G149"/>
-    <mergeCell ref="G151:G155"/>
-    <mergeCell ref="G157:G161"/>
-    <mergeCell ref="G163:G167"/>
-    <mergeCell ref="G169:G173"/>
-    <mergeCell ref="G175:G179"/>
-    <mergeCell ref="G181:G185"/>
-    <mergeCell ref="G187:G191"/>
-    <mergeCell ref="G193:G197"/>
-    <mergeCell ref="G199:G203"/>
-    <mergeCell ref="G205:G209"/>
-    <mergeCell ref="G211:G215"/>
-    <mergeCell ref="G217:G221"/>
-    <mergeCell ref="G223:G227"/>
-    <mergeCell ref="G229:G233"/>
-    <mergeCell ref="G235:G239"/>
-    <mergeCell ref="G241:G245"/>
-    <mergeCell ref="G247:G251"/>
-    <mergeCell ref="G253:G257"/>
-    <mergeCell ref="G259:G263"/>
-    <mergeCell ref="G265:G269"/>
-    <mergeCell ref="G271:G275"/>
-    <mergeCell ref="G277:G281"/>
-    <mergeCell ref="G283:G287"/>
-    <mergeCell ref="G289:G293"/>
-    <mergeCell ref="G295:G299"/>
-    <mergeCell ref="G301:G305"/>
-    <mergeCell ref="G307:G311"/>
-    <mergeCell ref="G313:G317"/>
-    <mergeCell ref="G319:G323"/>
-    <mergeCell ref="G325:G329"/>
-    <mergeCell ref="G331:G335"/>
-    <mergeCell ref="G337:G341"/>
-    <mergeCell ref="G343:G347"/>
-    <mergeCell ref="G349:G353"/>
-    <mergeCell ref="G355:G359"/>
-    <mergeCell ref="G361:G365"/>
-    <mergeCell ref="G367:G371"/>
-    <mergeCell ref="G373:G377"/>
-    <mergeCell ref="G379:G383"/>
-    <mergeCell ref="G385:G389"/>
-    <mergeCell ref="G391:G395"/>
-    <mergeCell ref="G397:G401"/>
-    <mergeCell ref="G403:G407"/>
-    <mergeCell ref="G409:G413"/>
-    <mergeCell ref="G415:G419"/>
-    <mergeCell ref="G421:G425"/>
-    <mergeCell ref="G427:G431"/>
-    <mergeCell ref="G433:G437"/>
-    <mergeCell ref="G439:G443"/>
-    <mergeCell ref="G445:G449"/>
-    <mergeCell ref="G451:G455"/>
-    <mergeCell ref="G457:G461"/>
-    <mergeCell ref="G463:G467"/>
-    <mergeCell ref="G469:G473"/>
-    <mergeCell ref="G475:G479"/>
-    <mergeCell ref="G481:G485"/>
-    <mergeCell ref="G487:G491"/>
-    <mergeCell ref="G493:G497"/>
-    <mergeCell ref="G499:G503"/>
-    <mergeCell ref="G505:G509"/>
-    <mergeCell ref="G511:G515"/>
-    <mergeCell ref="G517:G521"/>
-    <mergeCell ref="G523:G527"/>
-    <mergeCell ref="G529:G533"/>
-    <mergeCell ref="G535:G539"/>
-    <mergeCell ref="G541:G545"/>
-    <mergeCell ref="G547:G551"/>
-    <mergeCell ref="G553:G557"/>
-    <mergeCell ref="G559:G563"/>
-    <mergeCell ref="G565:G569"/>
-    <mergeCell ref="G571:G575"/>
-    <mergeCell ref="G577:G581"/>
-    <mergeCell ref="G583:G587"/>
-    <mergeCell ref="G589:G593"/>
-    <mergeCell ref="G595:G599"/>
-    <mergeCell ref="G601:G605"/>
-    <mergeCell ref="G607:G611"/>
-    <mergeCell ref="G613:G617"/>
-    <mergeCell ref="G619:G623"/>
-    <mergeCell ref="G625:G629"/>
-    <mergeCell ref="G631:G635"/>
-    <mergeCell ref="G637:G641"/>
-    <mergeCell ref="G643:G647"/>
-    <mergeCell ref="G649:G653"/>
-    <mergeCell ref="G655:G659"/>
-    <mergeCell ref="G661:G665"/>
-    <mergeCell ref="G667:G671"/>
-    <mergeCell ref="G673:G677"/>
-    <mergeCell ref="G679:G683"/>
-    <mergeCell ref="G685:G689"/>
-    <mergeCell ref="G691:G695"/>
-    <mergeCell ref="G697:G701"/>
-    <mergeCell ref="G703:G707"/>
-    <mergeCell ref="G709:G713"/>
-    <mergeCell ref="G715:G719"/>
-    <mergeCell ref="G721:G725"/>
-    <mergeCell ref="G727:G731"/>
-    <mergeCell ref="G733:G737"/>
-    <mergeCell ref="G739:G743"/>
-    <mergeCell ref="G745:G749"/>
-    <mergeCell ref="G751:G755"/>
-    <mergeCell ref="G757:G761"/>
-    <mergeCell ref="G763:G767"/>
-    <mergeCell ref="G769:G773"/>
-    <mergeCell ref="G775:G779"/>
-    <mergeCell ref="G781:G785"/>
-    <mergeCell ref="G787:G791"/>
-    <mergeCell ref="G793:G797"/>
-    <mergeCell ref="G799:G803"/>
-    <mergeCell ref="G805:G809"/>
-    <mergeCell ref="G811:G815"/>
-    <mergeCell ref="G817:G821"/>
-    <mergeCell ref="G823:G827"/>
-    <mergeCell ref="G829:G833"/>
-    <mergeCell ref="G835:G839"/>
-    <mergeCell ref="G841:G845"/>
-    <mergeCell ref="G847:G851"/>
-    <mergeCell ref="G853:G857"/>
-    <mergeCell ref="G859:G863"/>
-    <mergeCell ref="G865:G869"/>
-    <mergeCell ref="G871:G875"/>
-    <mergeCell ref="G877:G881"/>
-    <mergeCell ref="G883:G887"/>
-    <mergeCell ref="G889:G893"/>
-    <mergeCell ref="G895:G899"/>
-    <mergeCell ref="G901:G905"/>
-    <mergeCell ref="G907:G911"/>
-    <mergeCell ref="G913:G917"/>
-    <mergeCell ref="G985:G989"/>
-    <mergeCell ref="G991:G995"/>
-    <mergeCell ref="G997:G1001"/>
-    <mergeCell ref="G1003:G1007"/>
-    <mergeCell ref="G1009:G1013"/>
-    <mergeCell ref="G1015:G1019"/>
-    <mergeCell ref="G1021:G1025"/>
-    <mergeCell ref="G919:G923"/>
-    <mergeCell ref="G925:G929"/>
-    <mergeCell ref="G931:G935"/>
-    <mergeCell ref="G937:G941"/>
-    <mergeCell ref="G943:G947"/>
-    <mergeCell ref="G949:G953"/>
-    <mergeCell ref="G955:G959"/>
-    <mergeCell ref="G961:G965"/>
-    <mergeCell ref="G967:G971"/>
     <mergeCell ref="G1135:G1139"/>
     <mergeCell ref="G1141:G1145"/>
     <mergeCell ref="G1147:G1151"/>
@@ -23743,9 +23762,603 @@
     <mergeCell ref="G1075:G1079"/>
     <mergeCell ref="G973:G977"/>
     <mergeCell ref="G979:G983"/>
+    <mergeCell ref="G985:G989"/>
+    <mergeCell ref="G991:G995"/>
+    <mergeCell ref="G997:G1001"/>
+    <mergeCell ref="G1003:G1007"/>
+    <mergeCell ref="G1009:G1013"/>
+    <mergeCell ref="G1015:G1019"/>
+    <mergeCell ref="G1021:G1025"/>
+    <mergeCell ref="G919:G923"/>
+    <mergeCell ref="G925:G929"/>
+    <mergeCell ref="G931:G935"/>
+    <mergeCell ref="G937:G941"/>
+    <mergeCell ref="G943:G947"/>
+    <mergeCell ref="G949:G953"/>
+    <mergeCell ref="G955:G959"/>
+    <mergeCell ref="G961:G965"/>
+    <mergeCell ref="G967:G971"/>
+    <mergeCell ref="G865:G869"/>
+    <mergeCell ref="G871:G875"/>
+    <mergeCell ref="G877:G881"/>
+    <mergeCell ref="G883:G887"/>
+    <mergeCell ref="G889:G893"/>
+    <mergeCell ref="G895:G899"/>
+    <mergeCell ref="G901:G905"/>
+    <mergeCell ref="G907:G911"/>
+    <mergeCell ref="G913:G917"/>
+    <mergeCell ref="G811:G815"/>
+    <mergeCell ref="G817:G821"/>
+    <mergeCell ref="G823:G827"/>
+    <mergeCell ref="G829:G833"/>
+    <mergeCell ref="G835:G839"/>
+    <mergeCell ref="G841:G845"/>
+    <mergeCell ref="G847:G851"/>
+    <mergeCell ref="G853:G857"/>
+    <mergeCell ref="G859:G863"/>
+    <mergeCell ref="G757:G761"/>
+    <mergeCell ref="G763:G767"/>
+    <mergeCell ref="G769:G773"/>
+    <mergeCell ref="G775:G779"/>
+    <mergeCell ref="G781:G785"/>
+    <mergeCell ref="G787:G791"/>
+    <mergeCell ref="G793:G797"/>
+    <mergeCell ref="G799:G803"/>
+    <mergeCell ref="G805:G809"/>
+    <mergeCell ref="G703:G707"/>
+    <mergeCell ref="G709:G713"/>
+    <mergeCell ref="G715:G719"/>
+    <mergeCell ref="G721:G725"/>
+    <mergeCell ref="G727:G731"/>
+    <mergeCell ref="G733:G737"/>
+    <mergeCell ref="G739:G743"/>
+    <mergeCell ref="G745:G749"/>
+    <mergeCell ref="G751:G755"/>
+    <mergeCell ref="G649:G653"/>
+    <mergeCell ref="G655:G659"/>
+    <mergeCell ref="G661:G665"/>
+    <mergeCell ref="G667:G671"/>
+    <mergeCell ref="G673:G677"/>
+    <mergeCell ref="G679:G683"/>
+    <mergeCell ref="G685:G689"/>
+    <mergeCell ref="G691:G695"/>
+    <mergeCell ref="G697:G701"/>
+    <mergeCell ref="G595:G599"/>
+    <mergeCell ref="G601:G605"/>
+    <mergeCell ref="G607:G611"/>
+    <mergeCell ref="G613:G617"/>
+    <mergeCell ref="G619:G623"/>
+    <mergeCell ref="G625:G629"/>
+    <mergeCell ref="G631:G635"/>
+    <mergeCell ref="G637:G641"/>
+    <mergeCell ref="G643:G647"/>
+    <mergeCell ref="G541:G545"/>
+    <mergeCell ref="G547:G551"/>
+    <mergeCell ref="G553:G557"/>
+    <mergeCell ref="G559:G563"/>
+    <mergeCell ref="G565:G569"/>
+    <mergeCell ref="G571:G575"/>
+    <mergeCell ref="G577:G581"/>
+    <mergeCell ref="G583:G587"/>
+    <mergeCell ref="G589:G593"/>
+    <mergeCell ref="G487:G491"/>
+    <mergeCell ref="G493:G497"/>
+    <mergeCell ref="G499:G503"/>
+    <mergeCell ref="G505:G509"/>
+    <mergeCell ref="G511:G515"/>
+    <mergeCell ref="G517:G521"/>
+    <mergeCell ref="G523:G527"/>
+    <mergeCell ref="G529:G533"/>
+    <mergeCell ref="G535:G539"/>
+    <mergeCell ref="G433:G437"/>
+    <mergeCell ref="G439:G443"/>
+    <mergeCell ref="G445:G449"/>
+    <mergeCell ref="G451:G455"/>
+    <mergeCell ref="G457:G461"/>
+    <mergeCell ref="G463:G467"/>
+    <mergeCell ref="G469:G473"/>
+    <mergeCell ref="G475:G479"/>
+    <mergeCell ref="G481:G485"/>
+    <mergeCell ref="G379:G383"/>
+    <mergeCell ref="G385:G389"/>
+    <mergeCell ref="G391:G395"/>
+    <mergeCell ref="G397:G401"/>
+    <mergeCell ref="G403:G407"/>
+    <mergeCell ref="G409:G413"/>
+    <mergeCell ref="G415:G419"/>
+    <mergeCell ref="G421:G425"/>
+    <mergeCell ref="G427:G431"/>
+    <mergeCell ref="G325:G329"/>
+    <mergeCell ref="G331:G335"/>
+    <mergeCell ref="G337:G341"/>
+    <mergeCell ref="G343:G347"/>
+    <mergeCell ref="G349:G353"/>
+    <mergeCell ref="G355:G359"/>
+    <mergeCell ref="G361:G365"/>
+    <mergeCell ref="G367:G371"/>
+    <mergeCell ref="G373:G377"/>
+    <mergeCell ref="G271:G275"/>
+    <mergeCell ref="G277:G281"/>
+    <mergeCell ref="G283:G287"/>
+    <mergeCell ref="G289:G293"/>
+    <mergeCell ref="G295:G299"/>
+    <mergeCell ref="G301:G305"/>
+    <mergeCell ref="G307:G311"/>
+    <mergeCell ref="G313:G317"/>
+    <mergeCell ref="G319:G323"/>
+    <mergeCell ref="G217:G221"/>
+    <mergeCell ref="G223:G227"/>
+    <mergeCell ref="G229:G233"/>
+    <mergeCell ref="G235:G239"/>
+    <mergeCell ref="G241:G245"/>
+    <mergeCell ref="G247:G251"/>
+    <mergeCell ref="G253:G257"/>
+    <mergeCell ref="G259:G263"/>
+    <mergeCell ref="G265:G269"/>
+    <mergeCell ref="G163:G167"/>
+    <mergeCell ref="G169:G173"/>
+    <mergeCell ref="G175:G179"/>
+    <mergeCell ref="G181:G185"/>
+    <mergeCell ref="G187:G191"/>
+    <mergeCell ref="G193:G197"/>
+    <mergeCell ref="G199:G203"/>
+    <mergeCell ref="G205:G209"/>
+    <mergeCell ref="G211:G215"/>
+    <mergeCell ref="G109:G113"/>
+    <mergeCell ref="G115:G119"/>
+    <mergeCell ref="G121:G125"/>
+    <mergeCell ref="G127:G131"/>
+    <mergeCell ref="G133:G137"/>
+    <mergeCell ref="G139:G143"/>
+    <mergeCell ref="G145:G149"/>
+    <mergeCell ref="G151:G155"/>
+    <mergeCell ref="G157:G161"/>
+    <mergeCell ref="G55:G59"/>
+    <mergeCell ref="G61:G65"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="G73:G77"/>
+    <mergeCell ref="G79:G83"/>
+    <mergeCell ref="G85:G89"/>
+    <mergeCell ref="G91:G95"/>
+    <mergeCell ref="G97:G101"/>
+    <mergeCell ref="G103:G107"/>
+    <mergeCell ref="G1:G5"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G13:G17"/>
+    <mergeCell ref="G19:G23"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="A133:A137"/>
+    <mergeCell ref="A139:A143"/>
+    <mergeCell ref="A73:A77"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="A103:A107"/>
+    <mergeCell ref="A181:A185"/>
+    <mergeCell ref="A187:A191"/>
+    <mergeCell ref="A193:A197"/>
+    <mergeCell ref="A199:A203"/>
+    <mergeCell ref="A205:A209"/>
+    <mergeCell ref="A211:A215"/>
+    <mergeCell ref="A145:A149"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="A163:A167"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A175:A179"/>
+    <mergeCell ref="A253:A257"/>
+    <mergeCell ref="A259:A263"/>
+    <mergeCell ref="A265:A269"/>
+    <mergeCell ref="A271:A275"/>
+    <mergeCell ref="A277:A281"/>
+    <mergeCell ref="A283:A287"/>
+    <mergeCell ref="A217:A221"/>
+    <mergeCell ref="A223:A227"/>
+    <mergeCell ref="A229:A233"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A241:A245"/>
+    <mergeCell ref="A247:A251"/>
+    <mergeCell ref="A325:A329"/>
+    <mergeCell ref="A331:A335"/>
+    <mergeCell ref="A337:A341"/>
+    <mergeCell ref="A343:A347"/>
+    <mergeCell ref="A349:A353"/>
+    <mergeCell ref="A355:A359"/>
+    <mergeCell ref="A289:A293"/>
+    <mergeCell ref="A295:A299"/>
+    <mergeCell ref="A301:A305"/>
+    <mergeCell ref="A307:A311"/>
+    <mergeCell ref="A313:A317"/>
+    <mergeCell ref="A319:A323"/>
+    <mergeCell ref="A397:A401"/>
+    <mergeCell ref="A403:A407"/>
+    <mergeCell ref="A409:A413"/>
+    <mergeCell ref="A415:A419"/>
+    <mergeCell ref="A421:A425"/>
+    <mergeCell ref="A427:A431"/>
+    <mergeCell ref="A361:A365"/>
+    <mergeCell ref="A367:A371"/>
+    <mergeCell ref="A373:A377"/>
+    <mergeCell ref="A379:A383"/>
+    <mergeCell ref="A385:A389"/>
+    <mergeCell ref="A391:A395"/>
+    <mergeCell ref="A469:A473"/>
+    <mergeCell ref="A475:A479"/>
+    <mergeCell ref="A481:A485"/>
+    <mergeCell ref="A487:A491"/>
+    <mergeCell ref="A493:A497"/>
+    <mergeCell ref="A499:A503"/>
+    <mergeCell ref="A433:A437"/>
+    <mergeCell ref="A439:A443"/>
+    <mergeCell ref="A445:A449"/>
+    <mergeCell ref="A451:A455"/>
+    <mergeCell ref="A457:A461"/>
+    <mergeCell ref="A463:A467"/>
+    <mergeCell ref="A541:A545"/>
+    <mergeCell ref="A547:A551"/>
+    <mergeCell ref="A553:A557"/>
+    <mergeCell ref="A559:A563"/>
+    <mergeCell ref="A565:A569"/>
+    <mergeCell ref="A571:A575"/>
+    <mergeCell ref="A505:A509"/>
+    <mergeCell ref="A511:A515"/>
+    <mergeCell ref="A517:A521"/>
+    <mergeCell ref="A523:A527"/>
+    <mergeCell ref="A529:A533"/>
+    <mergeCell ref="A535:A539"/>
+    <mergeCell ref="A613:A617"/>
+    <mergeCell ref="A619:A623"/>
+    <mergeCell ref="A625:A629"/>
+    <mergeCell ref="A631:A635"/>
+    <mergeCell ref="A637:A641"/>
+    <mergeCell ref="A643:A647"/>
+    <mergeCell ref="A577:A581"/>
+    <mergeCell ref="A583:A587"/>
+    <mergeCell ref="A589:A593"/>
+    <mergeCell ref="A595:A599"/>
+    <mergeCell ref="A601:A605"/>
+    <mergeCell ref="A607:A611"/>
+    <mergeCell ref="A685:A689"/>
+    <mergeCell ref="A691:A695"/>
+    <mergeCell ref="A697:A701"/>
+    <mergeCell ref="A703:A707"/>
+    <mergeCell ref="A709:A713"/>
+    <mergeCell ref="A715:A719"/>
+    <mergeCell ref="A649:A653"/>
+    <mergeCell ref="A655:A659"/>
+    <mergeCell ref="A661:A665"/>
+    <mergeCell ref="A667:A671"/>
+    <mergeCell ref="A673:A677"/>
+    <mergeCell ref="A679:A683"/>
+    <mergeCell ref="A757:A761"/>
+    <mergeCell ref="A763:A767"/>
+    <mergeCell ref="A769:A773"/>
+    <mergeCell ref="A775:A779"/>
+    <mergeCell ref="A781:A785"/>
+    <mergeCell ref="A787:A791"/>
+    <mergeCell ref="A721:A725"/>
+    <mergeCell ref="A727:A731"/>
+    <mergeCell ref="A733:A737"/>
+    <mergeCell ref="A739:A743"/>
+    <mergeCell ref="A745:A749"/>
+    <mergeCell ref="A751:A755"/>
+    <mergeCell ref="A829:A833"/>
+    <mergeCell ref="A835:A839"/>
+    <mergeCell ref="A841:A845"/>
+    <mergeCell ref="A847:A851"/>
+    <mergeCell ref="A853:A857"/>
+    <mergeCell ref="A859:A863"/>
+    <mergeCell ref="A793:A797"/>
+    <mergeCell ref="A799:A803"/>
+    <mergeCell ref="A805:A809"/>
+    <mergeCell ref="A811:A815"/>
+    <mergeCell ref="A817:A821"/>
+    <mergeCell ref="A823:A827"/>
+    <mergeCell ref="A901:A905"/>
+    <mergeCell ref="A907:A911"/>
+    <mergeCell ref="A913:A917"/>
+    <mergeCell ref="A919:A923"/>
+    <mergeCell ref="A925:A929"/>
+    <mergeCell ref="A931:A935"/>
+    <mergeCell ref="A865:A869"/>
+    <mergeCell ref="A871:A875"/>
+    <mergeCell ref="A877:A881"/>
+    <mergeCell ref="A883:A887"/>
+    <mergeCell ref="A889:A893"/>
+    <mergeCell ref="A895:A899"/>
+    <mergeCell ref="A973:A977"/>
+    <mergeCell ref="A979:A983"/>
+    <mergeCell ref="A985:A989"/>
+    <mergeCell ref="A991:A995"/>
+    <mergeCell ref="A997:A1001"/>
+    <mergeCell ref="A1003:A1007"/>
+    <mergeCell ref="A937:A941"/>
+    <mergeCell ref="A943:A947"/>
+    <mergeCell ref="A949:A953"/>
+    <mergeCell ref="A955:A959"/>
+    <mergeCell ref="A961:A965"/>
+    <mergeCell ref="A967:A971"/>
+    <mergeCell ref="A1045:A1049"/>
+    <mergeCell ref="A1051:A1055"/>
+    <mergeCell ref="A1057:A1061"/>
+    <mergeCell ref="A1063:A1067"/>
+    <mergeCell ref="A1069:A1073"/>
+    <mergeCell ref="A1075:A1079"/>
+    <mergeCell ref="A1009:A1013"/>
+    <mergeCell ref="A1015:A1019"/>
+    <mergeCell ref="A1021:A1025"/>
+    <mergeCell ref="A1027:A1031"/>
+    <mergeCell ref="A1033:A1037"/>
+    <mergeCell ref="A1039:A1043"/>
+    <mergeCell ref="A1117:A1121"/>
+    <mergeCell ref="A1123:A1127"/>
+    <mergeCell ref="A1129:A1133"/>
+    <mergeCell ref="A1135:A1139"/>
+    <mergeCell ref="A1141:A1145"/>
+    <mergeCell ref="A1147:A1151"/>
+    <mergeCell ref="A1081:A1085"/>
+    <mergeCell ref="A1087:A1091"/>
+    <mergeCell ref="A1093:A1097"/>
+    <mergeCell ref="A1099:A1103"/>
+    <mergeCell ref="A1105:A1109"/>
+    <mergeCell ref="A1111:A1115"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="25.875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="30.875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="14" style="22" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="54" x14ac:dyDescent="0.15">
+      <c r="A2" s="22" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="54" x14ac:dyDescent="0.15">
+      <c r="B3" s="22" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="54" x14ac:dyDescent="0.15">
+      <c r="B4" s="22" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" s="22" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="22" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A10" s="22" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A11" s="22" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="A17" s="22" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="A18" s="22" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="A19" s="22" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A20" s="22" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="22" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B23" s="22" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B24" s="22" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="B25" s="22" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="B26" s="22" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="B27" s="22" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="22" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A31" s="22" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A32" s="22" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B34" s="22" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B35" s="22" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B37" s="22" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B38" s="22" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="22" t="s">
+        <v>609</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -24181,10 +24794,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:H136"/>
+  <dimension ref="A2:H161"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -24417,477 +25030,587 @@
     </row>
     <row r="37" spans="1:3" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A37" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="B37" s="24" t="s">
         <v>381</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A40" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>407</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>408</v>
-      </c>
       <c r="C40" s="25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A41" s="25"/>
       <c r="B41" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="C41" s="25" t="s">
         <v>409</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="25"/>
       <c r="B42" s="25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C42" s="25"/>
     </row>
     <row r="43" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A43" s="25"/>
       <c r="B43" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="C43" s="25" t="s">
         <v>413</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="24" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="54" x14ac:dyDescent="0.15">
       <c r="A47" s="24" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A48" s="24" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="54" x14ac:dyDescent="0.15">
       <c r="A49" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A50" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A52" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>421</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="24" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="24" t="s">
+        <v>424</v>
+      </c>
+      <c r="B56" s="24" t="s">
         <v>425</v>
-      </c>
-      <c r="B56" s="24" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A57" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A58" s="24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="24" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="54" x14ac:dyDescent="0.15">
       <c r="B62" s="24" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B63" s="24" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B64" s="24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B65" s="24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B66" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B68" s="24" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B69" s="25" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B70" s="25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="24" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B76" s="24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B77" s="24" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B78" s="24" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B79" s="24" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="24" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B81" s="24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B82" s="24" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B83" s="24" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="A84" s="24" t="s">
+        <v>471</v>
+      </c>
+      <c r="B84" s="24" t="s">
         <v>472</v>
-      </c>
-      <c r="B84" s="24" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A86" s="24" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="A87" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="81" x14ac:dyDescent="0.15">
       <c r="B88" s="24" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B89" s="24" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A90" s="24" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="A91" s="24" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B92" s="24" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B93" s="24" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B94" s="24" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A96" s="24" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A97" s="24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B98" s="24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B99" s="24" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B100" s="24" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A101" s="24" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B102" s="24" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B103" s="24" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B104" s="24" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A106" s="24" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B107" s="24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B108" s="24" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B109" s="24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B110" s="24" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" s="24" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B112" s="24" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B113" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B114" s="30" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B115" s="24" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A116" s="24" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="81" x14ac:dyDescent="0.15">
       <c r="B117" s="24" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B118" s="24" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B119" s="24" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A120" s="24" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B121" s="24" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B122" s="24" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B123" s="24" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A124" s="24" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B125" s="24" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B126" s="24" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B127" s="24" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A129" s="24" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A130" s="24" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B131" s="24" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B132" s="24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A133" s="24" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A134" s="24" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B135" s="24" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B136" s="24" t="s">
-        <v>541</v>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A138" s="24" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A139" s="24" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="B140" s="24" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="B141" s="24" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="B142" s="24" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A143" s="24" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A144" s="24" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="108" x14ac:dyDescent="0.15">
+      <c r="B145" s="24" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="B146" s="24" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A147" s="24" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="A148" s="24" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B149" s="24" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="B150" s="24" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A153" s="24" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A154" s="24" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="B155" s="24" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B156" s="24" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A157" s="24" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="B158" s="24" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B159" s="24" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="54" x14ac:dyDescent="0.15">
+      <c r="B160" s="24" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B161" s="24" t="s">
+        <v>627</v>
       </c>
     </row>
   </sheetData>
@@ -25202,22 +25925,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="1" max="1" width="36" style="28" customWidth="1"/>
     <col min="2" max="2" width="36.375" customWidth="1"/>
     <col min="3" max="3" width="36.25" customWidth="1"/>
     <col min="4" max="4" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="35" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -25228,7 +25951,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="35" t="s">
         <v>244</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -25239,7 +25962,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="35" t="s">
         <v>246</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -25253,7 +25976,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="35" t="s">
         <v>248</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -25268,7 +25991,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="35" t="s">
         <v>250</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -25283,7 +26006,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="35" t="s">
         <v>252</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -25297,7 +26020,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="35" t="s">
         <v>254</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -25310,10 +26033,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+    </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="35" t="s">
         <v>256</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -25327,7 +26054,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="35" t="s">
         <v>258</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -25341,7 +26068,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="35" t="s">
         <v>260</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -25355,7 +26082,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="35" t="s">
         <v>262</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -25369,7 +26096,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="35" t="s">
         <v>264</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -25383,7 +26110,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="35" t="s">
         <v>266</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -25396,16 +26123,22 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+    </row>
     <row r="19" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="35" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="36" t="s">
         <v>116</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -25416,7 +26149,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="37" t="s">
         <v>112</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -25427,7 +26160,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="38" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="21" t="s">
@@ -25437,25 +26170,25 @@
         <v>736251</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="35" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="39" t="s">
         <v>121</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>376</v>
+        <v>628</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>122</v>
       </c>
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A28" s="27" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="39" t="s">
         <v>119</v>
       </c>
       <c r="B28" s="27" t="s">
@@ -25465,17 +26198,17 @@
         <v>110</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A29" s="27"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="39"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A30" s="27" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="39" t="s">
         <v>164</v>
       </c>
       <c r="B30" s="27" t="s">
@@ -25488,8 +26221,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="39" t="s">
         <v>179</v>
       </c>
       <c r="B31" s="27" t="s">
@@ -25501,31 +26234,31 @@
       <c r="D31" s="27"/>
     </row>
     <row r="32" spans="1:6" ht="57" x14ac:dyDescent="0.15">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="39" t="s">
         <v>179</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>175</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D32" s="27"/>
       <c r="E32" s="27" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F32" s="27" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A33" s="27"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="39"/>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
     </row>
     <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="39" t="s">
         <v>118</v>
       </c>
       <c r="B34" s="27" t="s">
@@ -25536,49 +26269,45 @@
       </c>
       <c r="D34" s="27"/>
     </row>
-    <row r="35" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A35" s="27" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="39" t="s">
         <v>176</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>178</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D35" s="27"/>
     </row>
-    <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A36" s="27"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="39"/>
       <c r="B36" s="27"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
     </row>
-    <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A37" s="28"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
     </row>
-    <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A38" s="28"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
     </row>
-    <row r="39" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A39" s="28"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
     </row>
-    <row r="40" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A40" s="28"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
       <c r="D40" s="28"/>
     </row>
-    <row r="41" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="28" t="s">
         <v>268</v>
       </c>
@@ -25592,7 +26321,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="28" t="s">
         <v>269</v>
       </c>
@@ -25606,37 +26335,33 @@
         <v>279</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A43" s="28"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B43" s="28" t="s">
         <v>270</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A44" s="28"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
     </row>
-    <row r="45" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A45" s="28"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
     </row>
-    <row r="46" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A46" s="28"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
     </row>
-    <row r="47" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="28" t="s">
         <v>281</v>
       </c>
@@ -25646,29 +26371,45 @@
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
     </row>
-    <row r="48" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A48" s="28"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B48" s="28"/>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
     </row>
-    <row r="49" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A49" s="28"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B49" s="28"/>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
     </row>
-    <row r="50" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A50" s="28"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B50" s="28"/>
       <c r="C50" s="28"/>
       <c r="D50" s="28"/>
     </row>
-    <row r="51" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A51" s="28"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B51" s="28"/>
       <c r="C51" s="28"/>
       <c r="D51" s="28"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="28" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="28" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B54" s="28" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B55" s="28" t="s">
+        <v>632</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -25680,10 +26421,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:G44"/>
+  <dimension ref="A2:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -25765,10 +26506,10 @@
     </row>
     <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>378</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>379</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>334</v>
@@ -25780,10 +26521,10 @@
         <v>347</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -25926,105 +26667,160 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="81" x14ac:dyDescent="0.15">
       <c r="A24" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>383</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="162" x14ac:dyDescent="0.15">
       <c r="A25" s="24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="108" x14ac:dyDescent="0.15">
       <c r="A26" s="24" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A27" s="24" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="24" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="24" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="B31" s="24" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="B32" s="24" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B33" s="24" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B34" s="24" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="24" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B37" s="24" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B38" s="24" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" s="24" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="24" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="24" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B42" s="24" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B43" s="24" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B44" s="24" t="s">
-        <v>554</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" s="24" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" s="24" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B47" s="24" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="B48" s="24" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B49" s="24" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" s="24" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="A51" s="24" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B52" s="24" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B53" s="24" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B54" s="24" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B55" s="24" t="s">
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -26083,8 +26879,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -26122,170 +26918,170 @@
     </row>
     <row r="8" spans="1:2" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A8" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="81" x14ac:dyDescent="0.15">
       <c r="A9" s="25"/>
       <c r="B9" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="108" x14ac:dyDescent="0.15">
       <c r="A10" s="25"/>
       <c r="B10" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B11" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>394</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B14" s="24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="24" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="24" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="54" x14ac:dyDescent="0.15">
       <c r="A21" s="24" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="54" x14ac:dyDescent="0.15">
       <c r="A22" s="24" t="s">
+        <v>401</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>402</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B25" s="24" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="B26" s="24" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="24" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A32" s="24" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B33" s="24" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B34" s="24" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B35" s="24" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="24" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="A37" s="24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B38" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="27" x14ac:dyDescent="0.15">
       <c r="B39" s="24" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B40" s="24" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="24" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B44" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="54" x14ac:dyDescent="0.15">
       <c r="B45" s="24" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ok Signed-off-by: qingxue0606 <77055664@qq.com>
</commit_message>
<xml_diff>
--- a/音调练习.xlsx
+++ b/音调练习.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6540" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6540" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="练" sheetId="3" r:id="rId1"/>
@@ -3762,8 +3762,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:X1153"/>
   <sheetViews>
-    <sheetView topLeftCell="G25" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
@@ -24007,6 +24007,366 @@
     </row>
   </sheetData>
   <mergeCells count="384">
+    <mergeCell ref="A1117:A1121"/>
+    <mergeCell ref="A1123:A1127"/>
+    <mergeCell ref="A1129:A1133"/>
+    <mergeCell ref="A1135:A1139"/>
+    <mergeCell ref="A1141:A1145"/>
+    <mergeCell ref="A1147:A1151"/>
+    <mergeCell ref="A1081:A1085"/>
+    <mergeCell ref="A1087:A1091"/>
+    <mergeCell ref="A1093:A1097"/>
+    <mergeCell ref="A1099:A1103"/>
+    <mergeCell ref="A1105:A1109"/>
+    <mergeCell ref="A1111:A1115"/>
+    <mergeCell ref="A1045:A1049"/>
+    <mergeCell ref="A1051:A1055"/>
+    <mergeCell ref="A1057:A1061"/>
+    <mergeCell ref="A1063:A1067"/>
+    <mergeCell ref="A1069:A1073"/>
+    <mergeCell ref="A1075:A1079"/>
+    <mergeCell ref="A1009:A1013"/>
+    <mergeCell ref="A1015:A1019"/>
+    <mergeCell ref="A1021:A1025"/>
+    <mergeCell ref="A1027:A1031"/>
+    <mergeCell ref="A1033:A1037"/>
+    <mergeCell ref="A1039:A1043"/>
+    <mergeCell ref="A973:A977"/>
+    <mergeCell ref="A979:A983"/>
+    <mergeCell ref="A985:A989"/>
+    <mergeCell ref="A991:A995"/>
+    <mergeCell ref="A997:A1001"/>
+    <mergeCell ref="A1003:A1007"/>
+    <mergeCell ref="A937:A941"/>
+    <mergeCell ref="A943:A947"/>
+    <mergeCell ref="A949:A953"/>
+    <mergeCell ref="A955:A959"/>
+    <mergeCell ref="A961:A965"/>
+    <mergeCell ref="A967:A971"/>
+    <mergeCell ref="A901:A905"/>
+    <mergeCell ref="A907:A911"/>
+    <mergeCell ref="A913:A917"/>
+    <mergeCell ref="A919:A923"/>
+    <mergeCell ref="A925:A929"/>
+    <mergeCell ref="A931:A935"/>
+    <mergeCell ref="A865:A869"/>
+    <mergeCell ref="A871:A875"/>
+    <mergeCell ref="A877:A881"/>
+    <mergeCell ref="A883:A887"/>
+    <mergeCell ref="A889:A893"/>
+    <mergeCell ref="A895:A899"/>
+    <mergeCell ref="A829:A833"/>
+    <mergeCell ref="A835:A839"/>
+    <mergeCell ref="A841:A845"/>
+    <mergeCell ref="A847:A851"/>
+    <mergeCell ref="A853:A857"/>
+    <mergeCell ref="A859:A863"/>
+    <mergeCell ref="A793:A797"/>
+    <mergeCell ref="A799:A803"/>
+    <mergeCell ref="A805:A809"/>
+    <mergeCell ref="A811:A815"/>
+    <mergeCell ref="A817:A821"/>
+    <mergeCell ref="A823:A827"/>
+    <mergeCell ref="A757:A761"/>
+    <mergeCell ref="A763:A767"/>
+    <mergeCell ref="A769:A773"/>
+    <mergeCell ref="A775:A779"/>
+    <mergeCell ref="A781:A785"/>
+    <mergeCell ref="A787:A791"/>
+    <mergeCell ref="A721:A725"/>
+    <mergeCell ref="A727:A731"/>
+    <mergeCell ref="A733:A737"/>
+    <mergeCell ref="A739:A743"/>
+    <mergeCell ref="A745:A749"/>
+    <mergeCell ref="A751:A755"/>
+    <mergeCell ref="A685:A689"/>
+    <mergeCell ref="A691:A695"/>
+    <mergeCell ref="A697:A701"/>
+    <mergeCell ref="A703:A707"/>
+    <mergeCell ref="A709:A713"/>
+    <mergeCell ref="A715:A719"/>
+    <mergeCell ref="A649:A653"/>
+    <mergeCell ref="A655:A659"/>
+    <mergeCell ref="A661:A665"/>
+    <mergeCell ref="A667:A671"/>
+    <mergeCell ref="A673:A677"/>
+    <mergeCell ref="A679:A683"/>
+    <mergeCell ref="A613:A617"/>
+    <mergeCell ref="A619:A623"/>
+    <mergeCell ref="A625:A629"/>
+    <mergeCell ref="A631:A635"/>
+    <mergeCell ref="A637:A641"/>
+    <mergeCell ref="A643:A647"/>
+    <mergeCell ref="A577:A581"/>
+    <mergeCell ref="A583:A587"/>
+    <mergeCell ref="A589:A593"/>
+    <mergeCell ref="A595:A599"/>
+    <mergeCell ref="A601:A605"/>
+    <mergeCell ref="A607:A611"/>
+    <mergeCell ref="A541:A545"/>
+    <mergeCell ref="A547:A551"/>
+    <mergeCell ref="A553:A557"/>
+    <mergeCell ref="A559:A563"/>
+    <mergeCell ref="A565:A569"/>
+    <mergeCell ref="A571:A575"/>
+    <mergeCell ref="A505:A509"/>
+    <mergeCell ref="A511:A515"/>
+    <mergeCell ref="A517:A521"/>
+    <mergeCell ref="A523:A527"/>
+    <mergeCell ref="A529:A533"/>
+    <mergeCell ref="A535:A539"/>
+    <mergeCell ref="A469:A473"/>
+    <mergeCell ref="A475:A479"/>
+    <mergeCell ref="A481:A485"/>
+    <mergeCell ref="A487:A491"/>
+    <mergeCell ref="A493:A497"/>
+    <mergeCell ref="A499:A503"/>
+    <mergeCell ref="A433:A437"/>
+    <mergeCell ref="A439:A443"/>
+    <mergeCell ref="A445:A449"/>
+    <mergeCell ref="A451:A455"/>
+    <mergeCell ref="A457:A461"/>
+    <mergeCell ref="A463:A467"/>
+    <mergeCell ref="A397:A401"/>
+    <mergeCell ref="A403:A407"/>
+    <mergeCell ref="A409:A413"/>
+    <mergeCell ref="A415:A419"/>
+    <mergeCell ref="A421:A425"/>
+    <mergeCell ref="A427:A431"/>
+    <mergeCell ref="A361:A365"/>
+    <mergeCell ref="A367:A371"/>
+    <mergeCell ref="A373:A377"/>
+    <mergeCell ref="A379:A383"/>
+    <mergeCell ref="A385:A389"/>
+    <mergeCell ref="A391:A395"/>
+    <mergeCell ref="A325:A329"/>
+    <mergeCell ref="A331:A335"/>
+    <mergeCell ref="A337:A341"/>
+    <mergeCell ref="A343:A347"/>
+    <mergeCell ref="A349:A353"/>
+    <mergeCell ref="A355:A359"/>
+    <mergeCell ref="A289:A293"/>
+    <mergeCell ref="A295:A299"/>
+    <mergeCell ref="A301:A305"/>
+    <mergeCell ref="A307:A311"/>
+    <mergeCell ref="A313:A317"/>
+    <mergeCell ref="A319:A323"/>
+    <mergeCell ref="A253:A257"/>
+    <mergeCell ref="A259:A263"/>
+    <mergeCell ref="A265:A269"/>
+    <mergeCell ref="A271:A275"/>
+    <mergeCell ref="A277:A281"/>
+    <mergeCell ref="A283:A287"/>
+    <mergeCell ref="A217:A221"/>
+    <mergeCell ref="A223:A227"/>
+    <mergeCell ref="A229:A233"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A241:A245"/>
+    <mergeCell ref="A247:A251"/>
+    <mergeCell ref="A181:A185"/>
+    <mergeCell ref="A187:A191"/>
+    <mergeCell ref="A193:A197"/>
+    <mergeCell ref="A199:A203"/>
+    <mergeCell ref="A205:A209"/>
+    <mergeCell ref="A211:A215"/>
+    <mergeCell ref="A145:A149"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="A163:A167"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A175:A179"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="A133:A137"/>
+    <mergeCell ref="A139:A143"/>
+    <mergeCell ref="A73:A77"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="A103:A107"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="G1:G5"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G13:G17"/>
+    <mergeCell ref="G19:G23"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="G55:G59"/>
+    <mergeCell ref="G61:G65"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="G73:G77"/>
+    <mergeCell ref="G79:G83"/>
+    <mergeCell ref="G85:G89"/>
+    <mergeCell ref="G91:G95"/>
+    <mergeCell ref="G97:G101"/>
+    <mergeCell ref="G103:G107"/>
+    <mergeCell ref="G109:G113"/>
+    <mergeCell ref="G115:G119"/>
+    <mergeCell ref="G121:G125"/>
+    <mergeCell ref="G127:G131"/>
+    <mergeCell ref="G133:G137"/>
+    <mergeCell ref="G139:G143"/>
+    <mergeCell ref="G145:G149"/>
+    <mergeCell ref="G151:G155"/>
+    <mergeCell ref="G157:G161"/>
+    <mergeCell ref="G163:G167"/>
+    <mergeCell ref="G169:G173"/>
+    <mergeCell ref="G175:G179"/>
+    <mergeCell ref="G181:G185"/>
+    <mergeCell ref="G187:G191"/>
+    <mergeCell ref="G193:G197"/>
+    <mergeCell ref="G199:G203"/>
+    <mergeCell ref="G205:G209"/>
+    <mergeCell ref="G211:G215"/>
+    <mergeCell ref="G217:G221"/>
+    <mergeCell ref="G223:G227"/>
+    <mergeCell ref="G229:G233"/>
+    <mergeCell ref="G235:G239"/>
+    <mergeCell ref="G241:G245"/>
+    <mergeCell ref="G247:G251"/>
+    <mergeCell ref="G253:G257"/>
+    <mergeCell ref="G259:G263"/>
+    <mergeCell ref="G265:G269"/>
+    <mergeCell ref="G271:G275"/>
+    <mergeCell ref="G277:G281"/>
+    <mergeCell ref="G283:G287"/>
+    <mergeCell ref="G289:G293"/>
+    <mergeCell ref="G295:G299"/>
+    <mergeCell ref="G301:G305"/>
+    <mergeCell ref="G307:G311"/>
+    <mergeCell ref="G313:G317"/>
+    <mergeCell ref="G319:G323"/>
+    <mergeCell ref="G325:G329"/>
+    <mergeCell ref="G331:G335"/>
+    <mergeCell ref="G337:G341"/>
+    <mergeCell ref="G343:G347"/>
+    <mergeCell ref="G349:G353"/>
+    <mergeCell ref="G355:G359"/>
+    <mergeCell ref="G361:G365"/>
+    <mergeCell ref="G367:G371"/>
+    <mergeCell ref="G373:G377"/>
+    <mergeCell ref="G379:G383"/>
+    <mergeCell ref="G385:G389"/>
+    <mergeCell ref="G391:G395"/>
+    <mergeCell ref="G397:G401"/>
+    <mergeCell ref="G403:G407"/>
+    <mergeCell ref="G409:G413"/>
+    <mergeCell ref="G415:G419"/>
+    <mergeCell ref="G421:G425"/>
+    <mergeCell ref="G427:G431"/>
+    <mergeCell ref="G433:G437"/>
+    <mergeCell ref="G439:G443"/>
+    <mergeCell ref="G445:G449"/>
+    <mergeCell ref="G451:G455"/>
+    <mergeCell ref="G457:G461"/>
+    <mergeCell ref="G463:G467"/>
+    <mergeCell ref="G469:G473"/>
+    <mergeCell ref="G475:G479"/>
+    <mergeCell ref="G481:G485"/>
+    <mergeCell ref="G487:G491"/>
+    <mergeCell ref="G493:G497"/>
+    <mergeCell ref="G499:G503"/>
+    <mergeCell ref="G505:G509"/>
+    <mergeCell ref="G511:G515"/>
+    <mergeCell ref="G517:G521"/>
+    <mergeCell ref="G523:G527"/>
+    <mergeCell ref="G529:G533"/>
+    <mergeCell ref="G535:G539"/>
+    <mergeCell ref="G541:G545"/>
+    <mergeCell ref="G547:G551"/>
+    <mergeCell ref="G553:G557"/>
+    <mergeCell ref="G559:G563"/>
+    <mergeCell ref="G565:G569"/>
+    <mergeCell ref="G571:G575"/>
+    <mergeCell ref="G577:G581"/>
+    <mergeCell ref="G583:G587"/>
+    <mergeCell ref="G589:G593"/>
+    <mergeCell ref="G595:G599"/>
+    <mergeCell ref="G601:G605"/>
+    <mergeCell ref="G607:G611"/>
+    <mergeCell ref="G613:G617"/>
+    <mergeCell ref="G619:G623"/>
+    <mergeCell ref="G625:G629"/>
+    <mergeCell ref="G631:G635"/>
+    <mergeCell ref="G637:G641"/>
+    <mergeCell ref="G643:G647"/>
+    <mergeCell ref="G649:G653"/>
+    <mergeCell ref="G655:G659"/>
+    <mergeCell ref="G661:G665"/>
+    <mergeCell ref="G667:G671"/>
+    <mergeCell ref="G673:G677"/>
+    <mergeCell ref="G679:G683"/>
+    <mergeCell ref="G685:G689"/>
+    <mergeCell ref="G691:G695"/>
+    <mergeCell ref="G697:G701"/>
+    <mergeCell ref="G703:G707"/>
+    <mergeCell ref="G709:G713"/>
+    <mergeCell ref="G715:G719"/>
+    <mergeCell ref="G721:G725"/>
+    <mergeCell ref="G727:G731"/>
+    <mergeCell ref="G733:G737"/>
+    <mergeCell ref="G739:G743"/>
+    <mergeCell ref="G745:G749"/>
+    <mergeCell ref="G751:G755"/>
+    <mergeCell ref="G757:G761"/>
+    <mergeCell ref="G763:G767"/>
+    <mergeCell ref="G769:G773"/>
+    <mergeCell ref="G775:G779"/>
+    <mergeCell ref="G781:G785"/>
+    <mergeCell ref="G787:G791"/>
+    <mergeCell ref="G793:G797"/>
+    <mergeCell ref="G799:G803"/>
+    <mergeCell ref="G805:G809"/>
+    <mergeCell ref="G811:G815"/>
+    <mergeCell ref="G817:G821"/>
+    <mergeCell ref="G823:G827"/>
+    <mergeCell ref="G829:G833"/>
+    <mergeCell ref="G835:G839"/>
+    <mergeCell ref="G841:G845"/>
+    <mergeCell ref="G847:G851"/>
+    <mergeCell ref="G853:G857"/>
+    <mergeCell ref="G859:G863"/>
+    <mergeCell ref="G865:G869"/>
+    <mergeCell ref="G871:G875"/>
+    <mergeCell ref="G877:G881"/>
+    <mergeCell ref="G883:G887"/>
+    <mergeCell ref="G889:G893"/>
+    <mergeCell ref="G895:G899"/>
+    <mergeCell ref="G901:G905"/>
+    <mergeCell ref="G907:G911"/>
+    <mergeCell ref="G913:G917"/>
+    <mergeCell ref="G985:G989"/>
+    <mergeCell ref="G991:G995"/>
+    <mergeCell ref="G997:G1001"/>
+    <mergeCell ref="G1003:G1007"/>
+    <mergeCell ref="G1009:G1013"/>
+    <mergeCell ref="G1015:G1019"/>
+    <mergeCell ref="G1021:G1025"/>
+    <mergeCell ref="G919:G923"/>
+    <mergeCell ref="G925:G929"/>
+    <mergeCell ref="G931:G935"/>
+    <mergeCell ref="G937:G941"/>
+    <mergeCell ref="G943:G947"/>
+    <mergeCell ref="G949:G953"/>
+    <mergeCell ref="G955:G959"/>
+    <mergeCell ref="G961:G965"/>
+    <mergeCell ref="G967:G971"/>
     <mergeCell ref="G1135:G1139"/>
     <mergeCell ref="G1141:G1145"/>
     <mergeCell ref="G1147:G1151"/>
@@ -24031,366 +24391,6 @@
     <mergeCell ref="G1075:G1079"/>
     <mergeCell ref="G973:G977"/>
     <mergeCell ref="G979:G983"/>
-    <mergeCell ref="G985:G989"/>
-    <mergeCell ref="G991:G995"/>
-    <mergeCell ref="G997:G1001"/>
-    <mergeCell ref="G1003:G1007"/>
-    <mergeCell ref="G1009:G1013"/>
-    <mergeCell ref="G1015:G1019"/>
-    <mergeCell ref="G1021:G1025"/>
-    <mergeCell ref="G919:G923"/>
-    <mergeCell ref="G925:G929"/>
-    <mergeCell ref="G931:G935"/>
-    <mergeCell ref="G937:G941"/>
-    <mergeCell ref="G943:G947"/>
-    <mergeCell ref="G949:G953"/>
-    <mergeCell ref="G955:G959"/>
-    <mergeCell ref="G961:G965"/>
-    <mergeCell ref="G967:G971"/>
-    <mergeCell ref="G865:G869"/>
-    <mergeCell ref="G871:G875"/>
-    <mergeCell ref="G877:G881"/>
-    <mergeCell ref="G883:G887"/>
-    <mergeCell ref="G889:G893"/>
-    <mergeCell ref="G895:G899"/>
-    <mergeCell ref="G901:G905"/>
-    <mergeCell ref="G907:G911"/>
-    <mergeCell ref="G913:G917"/>
-    <mergeCell ref="G811:G815"/>
-    <mergeCell ref="G817:G821"/>
-    <mergeCell ref="G823:G827"/>
-    <mergeCell ref="G829:G833"/>
-    <mergeCell ref="G835:G839"/>
-    <mergeCell ref="G841:G845"/>
-    <mergeCell ref="G847:G851"/>
-    <mergeCell ref="G853:G857"/>
-    <mergeCell ref="G859:G863"/>
-    <mergeCell ref="G757:G761"/>
-    <mergeCell ref="G763:G767"/>
-    <mergeCell ref="G769:G773"/>
-    <mergeCell ref="G775:G779"/>
-    <mergeCell ref="G781:G785"/>
-    <mergeCell ref="G787:G791"/>
-    <mergeCell ref="G793:G797"/>
-    <mergeCell ref="G799:G803"/>
-    <mergeCell ref="G805:G809"/>
-    <mergeCell ref="G703:G707"/>
-    <mergeCell ref="G709:G713"/>
-    <mergeCell ref="G715:G719"/>
-    <mergeCell ref="G721:G725"/>
-    <mergeCell ref="G727:G731"/>
-    <mergeCell ref="G733:G737"/>
-    <mergeCell ref="G739:G743"/>
-    <mergeCell ref="G745:G749"/>
-    <mergeCell ref="G751:G755"/>
-    <mergeCell ref="G649:G653"/>
-    <mergeCell ref="G655:G659"/>
-    <mergeCell ref="G661:G665"/>
-    <mergeCell ref="G667:G671"/>
-    <mergeCell ref="G673:G677"/>
-    <mergeCell ref="G679:G683"/>
-    <mergeCell ref="G685:G689"/>
-    <mergeCell ref="G691:G695"/>
-    <mergeCell ref="G697:G701"/>
-    <mergeCell ref="G595:G599"/>
-    <mergeCell ref="G601:G605"/>
-    <mergeCell ref="G607:G611"/>
-    <mergeCell ref="G613:G617"/>
-    <mergeCell ref="G619:G623"/>
-    <mergeCell ref="G625:G629"/>
-    <mergeCell ref="G631:G635"/>
-    <mergeCell ref="G637:G641"/>
-    <mergeCell ref="G643:G647"/>
-    <mergeCell ref="G541:G545"/>
-    <mergeCell ref="G547:G551"/>
-    <mergeCell ref="G553:G557"/>
-    <mergeCell ref="G559:G563"/>
-    <mergeCell ref="G565:G569"/>
-    <mergeCell ref="G571:G575"/>
-    <mergeCell ref="G577:G581"/>
-    <mergeCell ref="G583:G587"/>
-    <mergeCell ref="G589:G593"/>
-    <mergeCell ref="G487:G491"/>
-    <mergeCell ref="G493:G497"/>
-    <mergeCell ref="G499:G503"/>
-    <mergeCell ref="G505:G509"/>
-    <mergeCell ref="G511:G515"/>
-    <mergeCell ref="G517:G521"/>
-    <mergeCell ref="G523:G527"/>
-    <mergeCell ref="G529:G533"/>
-    <mergeCell ref="G535:G539"/>
-    <mergeCell ref="G433:G437"/>
-    <mergeCell ref="G439:G443"/>
-    <mergeCell ref="G445:G449"/>
-    <mergeCell ref="G451:G455"/>
-    <mergeCell ref="G457:G461"/>
-    <mergeCell ref="G463:G467"/>
-    <mergeCell ref="G469:G473"/>
-    <mergeCell ref="G475:G479"/>
-    <mergeCell ref="G481:G485"/>
-    <mergeCell ref="G379:G383"/>
-    <mergeCell ref="G385:G389"/>
-    <mergeCell ref="G391:G395"/>
-    <mergeCell ref="G397:G401"/>
-    <mergeCell ref="G403:G407"/>
-    <mergeCell ref="G409:G413"/>
-    <mergeCell ref="G415:G419"/>
-    <mergeCell ref="G421:G425"/>
-    <mergeCell ref="G427:G431"/>
-    <mergeCell ref="G325:G329"/>
-    <mergeCell ref="G331:G335"/>
-    <mergeCell ref="G337:G341"/>
-    <mergeCell ref="G343:G347"/>
-    <mergeCell ref="G349:G353"/>
-    <mergeCell ref="G355:G359"/>
-    <mergeCell ref="G361:G365"/>
-    <mergeCell ref="G367:G371"/>
-    <mergeCell ref="G373:G377"/>
-    <mergeCell ref="G271:G275"/>
-    <mergeCell ref="G277:G281"/>
-    <mergeCell ref="G283:G287"/>
-    <mergeCell ref="G289:G293"/>
-    <mergeCell ref="G295:G299"/>
-    <mergeCell ref="G301:G305"/>
-    <mergeCell ref="G307:G311"/>
-    <mergeCell ref="G313:G317"/>
-    <mergeCell ref="G319:G323"/>
-    <mergeCell ref="G217:G221"/>
-    <mergeCell ref="G223:G227"/>
-    <mergeCell ref="G229:G233"/>
-    <mergeCell ref="G235:G239"/>
-    <mergeCell ref="G241:G245"/>
-    <mergeCell ref="G247:G251"/>
-    <mergeCell ref="G253:G257"/>
-    <mergeCell ref="G259:G263"/>
-    <mergeCell ref="G265:G269"/>
-    <mergeCell ref="G163:G167"/>
-    <mergeCell ref="G169:G173"/>
-    <mergeCell ref="G175:G179"/>
-    <mergeCell ref="G181:G185"/>
-    <mergeCell ref="G187:G191"/>
-    <mergeCell ref="G193:G197"/>
-    <mergeCell ref="G199:G203"/>
-    <mergeCell ref="G205:G209"/>
-    <mergeCell ref="G211:G215"/>
-    <mergeCell ref="G109:G113"/>
-    <mergeCell ref="G115:G119"/>
-    <mergeCell ref="G121:G125"/>
-    <mergeCell ref="G127:G131"/>
-    <mergeCell ref="G133:G137"/>
-    <mergeCell ref="G139:G143"/>
-    <mergeCell ref="G145:G149"/>
-    <mergeCell ref="G151:G155"/>
-    <mergeCell ref="G157:G161"/>
-    <mergeCell ref="G55:G59"/>
-    <mergeCell ref="G61:G65"/>
-    <mergeCell ref="G67:G71"/>
-    <mergeCell ref="G73:G77"/>
-    <mergeCell ref="G79:G83"/>
-    <mergeCell ref="G85:G89"/>
-    <mergeCell ref="G91:G95"/>
-    <mergeCell ref="G97:G101"/>
-    <mergeCell ref="G103:G107"/>
-    <mergeCell ref="G1:G5"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G13:G17"/>
-    <mergeCell ref="G19:G23"/>
-    <mergeCell ref="G25:G29"/>
-    <mergeCell ref="G31:G35"/>
-    <mergeCell ref="G37:G41"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="A115:A119"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="A133:A137"/>
-    <mergeCell ref="A139:A143"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="A103:A107"/>
-    <mergeCell ref="A181:A185"/>
-    <mergeCell ref="A187:A191"/>
-    <mergeCell ref="A193:A197"/>
-    <mergeCell ref="A199:A203"/>
-    <mergeCell ref="A205:A209"/>
-    <mergeCell ref="A211:A215"/>
-    <mergeCell ref="A145:A149"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="A157:A161"/>
-    <mergeCell ref="A163:A167"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A175:A179"/>
-    <mergeCell ref="A253:A257"/>
-    <mergeCell ref="A259:A263"/>
-    <mergeCell ref="A265:A269"/>
-    <mergeCell ref="A271:A275"/>
-    <mergeCell ref="A277:A281"/>
-    <mergeCell ref="A283:A287"/>
-    <mergeCell ref="A217:A221"/>
-    <mergeCell ref="A223:A227"/>
-    <mergeCell ref="A229:A233"/>
-    <mergeCell ref="A235:A239"/>
-    <mergeCell ref="A241:A245"/>
-    <mergeCell ref="A247:A251"/>
-    <mergeCell ref="A325:A329"/>
-    <mergeCell ref="A331:A335"/>
-    <mergeCell ref="A337:A341"/>
-    <mergeCell ref="A343:A347"/>
-    <mergeCell ref="A349:A353"/>
-    <mergeCell ref="A355:A359"/>
-    <mergeCell ref="A289:A293"/>
-    <mergeCell ref="A295:A299"/>
-    <mergeCell ref="A301:A305"/>
-    <mergeCell ref="A307:A311"/>
-    <mergeCell ref="A313:A317"/>
-    <mergeCell ref="A319:A323"/>
-    <mergeCell ref="A397:A401"/>
-    <mergeCell ref="A403:A407"/>
-    <mergeCell ref="A409:A413"/>
-    <mergeCell ref="A415:A419"/>
-    <mergeCell ref="A421:A425"/>
-    <mergeCell ref="A427:A431"/>
-    <mergeCell ref="A361:A365"/>
-    <mergeCell ref="A367:A371"/>
-    <mergeCell ref="A373:A377"/>
-    <mergeCell ref="A379:A383"/>
-    <mergeCell ref="A385:A389"/>
-    <mergeCell ref="A391:A395"/>
-    <mergeCell ref="A469:A473"/>
-    <mergeCell ref="A475:A479"/>
-    <mergeCell ref="A481:A485"/>
-    <mergeCell ref="A487:A491"/>
-    <mergeCell ref="A493:A497"/>
-    <mergeCell ref="A499:A503"/>
-    <mergeCell ref="A433:A437"/>
-    <mergeCell ref="A439:A443"/>
-    <mergeCell ref="A445:A449"/>
-    <mergeCell ref="A451:A455"/>
-    <mergeCell ref="A457:A461"/>
-    <mergeCell ref="A463:A467"/>
-    <mergeCell ref="A541:A545"/>
-    <mergeCell ref="A547:A551"/>
-    <mergeCell ref="A553:A557"/>
-    <mergeCell ref="A559:A563"/>
-    <mergeCell ref="A565:A569"/>
-    <mergeCell ref="A571:A575"/>
-    <mergeCell ref="A505:A509"/>
-    <mergeCell ref="A511:A515"/>
-    <mergeCell ref="A517:A521"/>
-    <mergeCell ref="A523:A527"/>
-    <mergeCell ref="A529:A533"/>
-    <mergeCell ref="A535:A539"/>
-    <mergeCell ref="A613:A617"/>
-    <mergeCell ref="A619:A623"/>
-    <mergeCell ref="A625:A629"/>
-    <mergeCell ref="A631:A635"/>
-    <mergeCell ref="A637:A641"/>
-    <mergeCell ref="A643:A647"/>
-    <mergeCell ref="A577:A581"/>
-    <mergeCell ref="A583:A587"/>
-    <mergeCell ref="A589:A593"/>
-    <mergeCell ref="A595:A599"/>
-    <mergeCell ref="A601:A605"/>
-    <mergeCell ref="A607:A611"/>
-    <mergeCell ref="A685:A689"/>
-    <mergeCell ref="A691:A695"/>
-    <mergeCell ref="A697:A701"/>
-    <mergeCell ref="A703:A707"/>
-    <mergeCell ref="A709:A713"/>
-    <mergeCell ref="A715:A719"/>
-    <mergeCell ref="A649:A653"/>
-    <mergeCell ref="A655:A659"/>
-    <mergeCell ref="A661:A665"/>
-    <mergeCell ref="A667:A671"/>
-    <mergeCell ref="A673:A677"/>
-    <mergeCell ref="A679:A683"/>
-    <mergeCell ref="A757:A761"/>
-    <mergeCell ref="A763:A767"/>
-    <mergeCell ref="A769:A773"/>
-    <mergeCell ref="A775:A779"/>
-    <mergeCell ref="A781:A785"/>
-    <mergeCell ref="A787:A791"/>
-    <mergeCell ref="A721:A725"/>
-    <mergeCell ref="A727:A731"/>
-    <mergeCell ref="A733:A737"/>
-    <mergeCell ref="A739:A743"/>
-    <mergeCell ref="A745:A749"/>
-    <mergeCell ref="A751:A755"/>
-    <mergeCell ref="A829:A833"/>
-    <mergeCell ref="A835:A839"/>
-    <mergeCell ref="A841:A845"/>
-    <mergeCell ref="A847:A851"/>
-    <mergeCell ref="A853:A857"/>
-    <mergeCell ref="A859:A863"/>
-    <mergeCell ref="A793:A797"/>
-    <mergeCell ref="A799:A803"/>
-    <mergeCell ref="A805:A809"/>
-    <mergeCell ref="A811:A815"/>
-    <mergeCell ref="A817:A821"/>
-    <mergeCell ref="A823:A827"/>
-    <mergeCell ref="A901:A905"/>
-    <mergeCell ref="A907:A911"/>
-    <mergeCell ref="A913:A917"/>
-    <mergeCell ref="A919:A923"/>
-    <mergeCell ref="A925:A929"/>
-    <mergeCell ref="A931:A935"/>
-    <mergeCell ref="A865:A869"/>
-    <mergeCell ref="A871:A875"/>
-    <mergeCell ref="A877:A881"/>
-    <mergeCell ref="A883:A887"/>
-    <mergeCell ref="A889:A893"/>
-    <mergeCell ref="A895:A899"/>
-    <mergeCell ref="A973:A977"/>
-    <mergeCell ref="A979:A983"/>
-    <mergeCell ref="A985:A989"/>
-    <mergeCell ref="A991:A995"/>
-    <mergeCell ref="A997:A1001"/>
-    <mergeCell ref="A1003:A1007"/>
-    <mergeCell ref="A937:A941"/>
-    <mergeCell ref="A943:A947"/>
-    <mergeCell ref="A949:A953"/>
-    <mergeCell ref="A955:A959"/>
-    <mergeCell ref="A961:A965"/>
-    <mergeCell ref="A967:A971"/>
-    <mergeCell ref="A1045:A1049"/>
-    <mergeCell ref="A1051:A1055"/>
-    <mergeCell ref="A1057:A1061"/>
-    <mergeCell ref="A1063:A1067"/>
-    <mergeCell ref="A1069:A1073"/>
-    <mergeCell ref="A1075:A1079"/>
-    <mergeCell ref="A1009:A1013"/>
-    <mergeCell ref="A1015:A1019"/>
-    <mergeCell ref="A1021:A1025"/>
-    <mergeCell ref="A1027:A1031"/>
-    <mergeCell ref="A1033:A1037"/>
-    <mergeCell ref="A1039:A1043"/>
-    <mergeCell ref="A1117:A1121"/>
-    <mergeCell ref="A1123:A1127"/>
-    <mergeCell ref="A1129:A1133"/>
-    <mergeCell ref="A1135:A1139"/>
-    <mergeCell ref="A1141:A1145"/>
-    <mergeCell ref="A1147:A1151"/>
-    <mergeCell ref="A1081:A1085"/>
-    <mergeCell ref="A1087:A1091"/>
-    <mergeCell ref="A1093:A1097"/>
-    <mergeCell ref="A1099:A1103"/>
-    <mergeCell ref="A1105:A1109"/>
-    <mergeCell ref="A1111:A1115"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24401,8 +24401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -25901,8 +25901,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -26206,8 +26206,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:B70"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>

</xml_diff>